<commit_message>
update tabel di tugas5 dan latihan membuat tabel diagram
</commit_message>
<xml_diff>
--- a/tugas_mysql/tugas5/tugas5.xlsx
+++ b/tugas_mysql/tugas5/tugas5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\QUERY_DBSIB5\tugas_mysql\tugas5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A1C4FD-A0C3-4FA9-87BB-2A01F0D39BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56370A87-2F2C-4778-AD61-7DCB469C5EF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AE12F976-3553-4775-9D03-2B6E84AA1572}"/>
+    <workbookView xWindow="696" yWindow="1944" windowWidth="17280" windowHeight="8964" xr2:uid="{AE12F976-3553-4775-9D03-2B6E84AA1572}"/>
   </bookViews>
   <sheets>
     <sheet name="Lembar1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="53">
   <si>
     <t>No</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>Tabel 3NF</t>
+  </si>
+  <si>
+    <t>Id</t>
   </si>
 </sst>
 </file>
@@ -217,7 +220,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -240,11 +243,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -258,6 +270,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{943A6BDB-97A6-4AE8-BE7D-C43A64728E84}">
-  <dimension ref="B3:Q54"/>
+  <dimension ref="B3:Q55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1139,6 +1152,7 @@
       <c r="G36" t="s">
         <v>43</v>
       </c>
+      <c r="M36" s="5"/>
       <c r="N36" t="s">
         <v>46</v>
       </c>
@@ -1168,6 +1182,9 @@
       <c r="K37" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="M37" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="N37" s="1" t="s">
         <v>45</v>
       </c>
@@ -1200,6 +1217,9 @@
       <c r="K38" s="4">
         <v>45211</v>
       </c>
+      <c r="M38" s="2">
+        <v>1</v>
+      </c>
       <c r="N38" s="2">
         <v>1</v>
       </c>
@@ -1232,6 +1252,9 @@
       <c r="K39" s="4">
         <v>45212</v>
       </c>
+      <c r="M39" s="2">
+        <v>2</v>
+      </c>
       <c r="N39" s="2">
         <v>2</v>
       </c>
@@ -1263,6 +1286,9 @@
       </c>
       <c r="K40" s="4">
         <v>45213</v>
+      </c>
+      <c r="M40" s="2">
+        <v>3</v>
       </c>
       <c r="N40" s="2">
         <v>3</v>
@@ -1518,7 +1544,7 @@
         <v>10000000</v>
       </c>
     </row>
-    <row r="49" spans="14:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="7:17" x14ac:dyDescent="0.3">
       <c r="N49" s="2">
         <v>5</v>
       </c>
@@ -1532,7 +1558,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="50" spans="14:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="7:17" x14ac:dyDescent="0.3">
       <c r="N50" s="2">
         <v>6</v>
       </c>
@@ -1546,7 +1572,10 @@
         <v>115000</v>
       </c>
     </row>
-    <row r="51" spans="14:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="7:17" x14ac:dyDescent="0.3">
+      <c r="G51" t="s">
+        <v>41</v>
+      </c>
       <c r="N51" s="2">
         <v>7</v>
       </c>
@@ -1560,7 +1589,13 @@
         <v>7000000</v>
       </c>
     </row>
-    <row r="52" spans="14:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="7:17" x14ac:dyDescent="0.3">
+      <c r="G52" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="N52" s="2">
         <v>8</v>
       </c>
@@ -1574,7 +1609,13 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="53" spans="14:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="7:17" x14ac:dyDescent="0.3">
+      <c r="G53" s="2">
+        <v>1</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="N53" s="2">
         <v>9</v>
       </c>
@@ -1588,7 +1629,13 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="54" spans="14:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="7:17" x14ac:dyDescent="0.3">
+      <c r="G54" s="2">
+        <v>2</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="N54" s="2">
         <v>10</v>
       </c>
@@ -1600,6 +1647,14 @@
       </c>
       <c r="Q54" s="3">
         <v>500000</v>
+      </c>
+    </row>
+    <row r="55" spans="7:17" x14ac:dyDescent="0.3">
+      <c r="G55" s="2">
+        <v>3</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
perbaikan tabel tugas 5 dan mengumpulkan tugas 6
</commit_message>
<xml_diff>
--- a/tugas_mysql/tugas5/tugas5.xlsx
+++ b/tugas_mysql/tugas5/tugas5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\QUERY_DBSIB5\tugas_mysql\tugas5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56370A87-2F2C-4778-AD61-7DCB469C5EF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C091C06-4DB4-474A-BB3D-36378D9A2CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="696" yWindow="1944" windowWidth="17280" windowHeight="8964" xr2:uid="{AE12F976-3553-4775-9D03-2B6E84AA1572}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AE12F976-3553-4775-9D03-2B6E84AA1572}"/>
   </bookViews>
   <sheets>
     <sheet name="Lembar1" sheetId="1" r:id="rId1"/>
@@ -585,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{943A6BDB-97A6-4AE8-BE7D-C43A64728E84}">
-  <dimension ref="B3:Q55"/>
+  <dimension ref="B3:L64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53:E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1140,24 +1140,20 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>42</v>
       </c>
       <c r="G36" t="s">
         <v>43</v>
       </c>
-      <c r="M36" s="5"/>
-      <c r="N36" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
         <v>50</v>
       </c>
@@ -1182,17 +1178,8 @@
       <c r="K37" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M37" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="N37" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="O37" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="2:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B38" s="2">
         <v>1</v>
       </c>
@@ -1217,17 +1204,8 @@
       <c r="K38" s="4">
         <v>45211</v>
       </c>
-      <c r="M38" s="2">
-        <v>1</v>
-      </c>
-      <c r="N38" s="2">
-        <v>1</v>
-      </c>
-      <c r="O38" s="3">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B39" s="2">
         <v>2</v>
       </c>
@@ -1252,17 +1230,8 @@
       <c r="K39" s="4">
         <v>45212</v>
       </c>
-      <c r="M39" s="2">
-        <v>2</v>
-      </c>
-      <c r="N39" s="2">
-        <v>2</v>
-      </c>
-      <c r="O39" s="3">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B40" s="2">
         <v>3</v>
       </c>
@@ -1287,17 +1256,8 @@
       <c r="K40" s="4">
         <v>45213</v>
       </c>
-      <c r="M40" s="2">
-        <v>3</v>
-      </c>
-      <c r="N40" s="2">
-        <v>3</v>
-      </c>
-      <c r="O40" s="3">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B41" s="2">
         <v>4</v>
       </c>
@@ -1323,7 +1283,7 @@
         <v>45214</v>
       </c>
     </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B42" s="2">
         <v>5</v>
       </c>
@@ -1349,7 +1309,7 @@
         <v>45215</v>
       </c>
     </row>
-    <row r="43" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B43" s="2">
         <v>6</v>
       </c>
@@ -1374,11 +1334,8 @@
       <c r="K43" s="4">
         <v>45216</v>
       </c>
-      <c r="N43" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="44" spans="2:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B44" s="2">
         <v>7</v>
       </c>
@@ -1403,20 +1360,8 @@
       <c r="K44" s="4">
         <v>45217</v>
       </c>
-      <c r="N44" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="O44" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="P44" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q44" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="2:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B45" s="2">
         <v>8</v>
       </c>
@@ -1441,20 +1386,8 @@
       <c r="K45" s="4">
         <v>45218</v>
       </c>
-      <c r="N45" s="2">
-        <v>1</v>
-      </c>
-      <c r="O45" s="2">
-        <v>1</v>
-      </c>
-      <c r="P45" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q45" s="3">
-        <v>2000000</v>
-      </c>
-    </row>
-    <row r="46" spans="2:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B46" s="2">
         <v>9</v>
       </c>
@@ -1479,20 +1412,8 @@
       <c r="K46" s="4">
         <v>45219</v>
       </c>
-      <c r="N46" s="2">
-        <v>2</v>
-      </c>
-      <c r="O46" s="2">
-        <v>2</v>
-      </c>
-      <c r="P46" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q46" s="3">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="47" spans="2:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B47" s="2">
         <v>10</v>
       </c>
@@ -1517,144 +1438,235 @@
       <c r="K47" s="4">
         <v>45220</v>
       </c>
-      <c r="N47" s="2">
-        <v>3</v>
-      </c>
-      <c r="O47" s="2">
-        <v>3</v>
-      </c>
-      <c r="P47" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q47" s="3">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="48" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="N48" s="2">
-        <v>4</v>
-      </c>
-      <c r="O48" s="2">
-        <v>4</v>
-      </c>
-      <c r="P48" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q48" s="3">
-        <v>10000000</v>
-      </c>
-    </row>
-    <row r="49" spans="7:17" x14ac:dyDescent="0.3">
-      <c r="N49" s="2">
-        <v>5</v>
-      </c>
-      <c r="O49" s="2">
-        <v>5</v>
-      </c>
-      <c r="P49" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q49" s="3">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="50" spans="7:17" x14ac:dyDescent="0.3">
-      <c r="N50" s="2">
-        <v>6</v>
-      </c>
-      <c r="O50" s="2">
-        <v>6</v>
-      </c>
-      <c r="P50" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q50" s="3">
-        <v>115000</v>
-      </c>
-    </row>
-    <row r="51" spans="7:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.3">
       <c r="G51" t="s">
         <v>41</v>
       </c>
-      <c r="N51" s="2">
-        <v>7</v>
-      </c>
-      <c r="O51" s="2">
-        <v>7</v>
-      </c>
-      <c r="P51" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q51" s="3">
-        <v>7000000</v>
-      </c>
-    </row>
-    <row r="52" spans="7:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.3">
       <c r="G52" s="1" t="s">
         <v>45</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="N52" s="2">
-        <v>8</v>
-      </c>
-      <c r="O52" s="2">
-        <v>8</v>
-      </c>
-      <c r="P52" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q52" s="3">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="53" spans="7:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>47</v>
+      </c>
       <c r="G53" s="2">
         <v>1</v>
       </c>
       <c r="H53" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="N53" s="2">
+      <c r="J53" s="5"/>
+      <c r="K53" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B54" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="O53" s="2">
-        <v>9</v>
-      </c>
-      <c r="P53" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q53" s="3">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="54" spans="7:17" x14ac:dyDescent="0.3">
+      <c r="E54" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="G54" s="2">
         <v>2</v>
       </c>
       <c r="H54" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="N54" s="2">
-        <v>10</v>
-      </c>
-      <c r="O54" s="2">
-        <v>10</v>
-      </c>
-      <c r="P54" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q54" s="3">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="55" spans="7:17" x14ac:dyDescent="0.3">
+      <c r="J54" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L54" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B55" s="2">
+        <v>1</v>
+      </c>
+      <c r="C55" s="2">
+        <v>1</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E55" s="3">
+        <v>2000000</v>
+      </c>
       <c r="G55" s="2">
         <v>3</v>
       </c>
       <c r="H55" s="2" t="s">
         <v>31</v>
+      </c>
+      <c r="J55" s="2">
+        <v>1</v>
+      </c>
+      <c r="K55" s="2">
+        <v>1</v>
+      </c>
+      <c r="L55" s="3">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B56" s="2">
+        <v>2</v>
+      </c>
+      <c r="C56" s="2">
+        <v>2</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E56" s="3">
+        <v>5000</v>
+      </c>
+      <c r="J56" s="2">
+        <v>2</v>
+      </c>
+      <c r="K56" s="2">
+        <v>2</v>
+      </c>
+      <c r="L56" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B57" s="2">
+        <v>3</v>
+      </c>
+      <c r="C57" s="2">
+        <v>3</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E57" s="3">
+        <v>50000</v>
+      </c>
+      <c r="J57" s="2">
+        <v>3</v>
+      </c>
+      <c r="K57" s="2">
+        <v>3</v>
+      </c>
+      <c r="L57" s="3">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="58" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B58" s="2">
+        <v>4</v>
+      </c>
+      <c r="C58" s="2">
+        <v>4</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E58" s="3">
+        <v>10000000</v>
+      </c>
+    </row>
+    <row r="59" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B59" s="2">
+        <v>5</v>
+      </c>
+      <c r="C59" s="2">
+        <v>5</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E59" s="3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="60" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B60" s="2">
+        <v>6</v>
+      </c>
+      <c r="C60" s="2">
+        <v>6</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E60" s="3">
+        <v>115000</v>
+      </c>
+    </row>
+    <row r="61" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B61" s="2">
+        <v>7</v>
+      </c>
+      <c r="C61" s="2">
+        <v>7</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E61" s="3">
+        <v>7000000</v>
+      </c>
+    </row>
+    <row r="62" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B62" s="2">
+        <v>8</v>
+      </c>
+      <c r="C62" s="2">
+        <v>8</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E62" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="63" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B63" s="2">
+        <v>9</v>
+      </c>
+      <c r="C63" s="2">
+        <v>9</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E63" s="3">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="64" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B64" s="2">
+        <v>10</v>
+      </c>
+      <c r="C64" s="2">
+        <v>10</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E64" s="3">
+        <v>500000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>